<commit_message>
✨ feat: add camera stream manager and config
</commit_message>
<xml_diff>
--- a/cameras.xlsx
+++ b/cameras.xlsx
@@ -1,20 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusta\code\local-cameras-view\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B13B06-F05A-4BF6-BDAD-9DB89A648F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Plan1"/>
+    <sheet name="Cameras" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Nome</t>
   </si>
@@ -38,15 +45,40 @@
   </si>
   <si>
     <t>123.45.67.8</t>
+  </si>
+  <si>
+    <t>Marca</t>
+  </si>
+  <si>
+    <t>Marcas</t>
+  </si>
+  <si>
+    <t>HIKVISION</t>
+  </si>
+  <si>
+    <t>EZVIZ</t>
+  </si>
+  <si>
+    <t>INTELBRAS</t>
+  </si>
+  <si>
+    <t>WEBCAM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -74,23 +106,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -101,10 +131,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -142,71 +172,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -234,7 +264,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -257,11 +287,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -270,13 +300,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -286,7 +316,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -295,7 +325,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -304,7 +334,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -312,10 +342,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -380,23 +410,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="2" width="8.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="7.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="8.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="11.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -409,22 +441,83 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CEEFD8B4-83B4-4FB3-ADBC-DC34070E8C50}">
+          <x14:formula1>
+            <xm:f>Data!$A$2:$A$1048576</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2532B59E-234D-4402-943A-DE70936D968E}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
⚡️ optmize stream performance
</commit_message>
<xml_diff>
--- a/cameras.xlsx
+++ b/cameras.xlsx
@@ -1,85 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusta\code\local-cameras-view\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B13B06-F05A-4BF6-BDAD-9DB89A648F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="Cameras" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
-  <si>
-    <t>Nome</t>
-  </si>
-  <si>
-    <t>Usuário</t>
-  </si>
-  <si>
-    <t>Senha</t>
-  </si>
-  <si>
-    <t>IP</t>
-  </si>
-  <si>
-    <t>Câmera 1</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>123.45.67.8</t>
-  </si>
-  <si>
-    <t>Marca</t>
-  </si>
-  <si>
-    <t>Marcas</t>
-  </si>
-  <si>
-    <t>HIKVISION</t>
-  </si>
-  <si>
-    <t>EZVIZ</t>
-  </si>
-  <si>
-    <t>INTELBRAS</t>
-  </si>
-  <si>
-    <t>WEBCAM</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -106,23 +65,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -137,28 +87,28 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="0000FF"/>
@@ -260,6 +210,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
@@ -270,31 +221,27 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="51000"/>
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="94000"/>
-                <a:satMod val="135000"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="9500"/>
+              <a:shade val="95000"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
@@ -316,7 +263,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -374,7 +321,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="20000"/>
+                <a:shade val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -387,12 +334,13 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
+                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -404,120 +352,133 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Nome</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Usuário</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Senha</v>
+      </c>
+      <c r="D1" t="str">
+        <v>IP</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Marca</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Câmera 1</v>
+      </c>
+      <c r="B2" t="str">
+        <v>admin</v>
+      </c>
+      <c r="C2" t="str">
+        <v>test</v>
+      </c>
+      <c r="D2" t="str">
+        <v>123.45.67.8</v>
+      </c>
+      <c r="E2" t="str">
+        <v>WEBCAM</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CEEFD8B4-83B4-4FB3-ADBC-DC34070E8C50}">
-          <x14:formula1>
-            <xm:f>Data!$A$2:$A$1048576</xm:f>
-          </x14:formula1>
-          <xm:sqref>E2:E1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2532B59E-234D-4402-943A-DE70936D968E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>13</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Marcas</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>HIKVISION</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>EZVIZ</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>INTELBRAS</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>WEBCAM</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:A5"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>